<commit_message>
손서연 # 06.16 05:33
1. chatbot
- load text form
- answer form
</commit_message>
<xml_diff>
--- a/train_data/train_data_q&a.xlsx
+++ b/train_data/train_data_q&a.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevRoot\TeamProj2\train_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevRoot\new\TeamProj2\train_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B47F7-ED03-4E97-9264-D949E1770CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718A37F3-5A80-4DFE-9AAC-7A67FA614231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="396" windowWidth="19836" windowHeight="11556" xr2:uid="{692F1389-EF55-407A-9BB7-949C0F708E50}"/>
+    <workbookView xWindow="1080" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{692F1389-EF55-407A-9BB7-949C0F708E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>개체명</t>
   </si>
@@ -1033,6 +1033,85 @@
   </si>
   <si>
     <t>옵션 및 수량을 선택해주세요</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>고객님의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>취향에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>맞춰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>골라봤어요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>. ,</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1585,13 +1664,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0132C9F-F541-4990-8737-8F12103C4879}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.8" thickBot="1">
+    <row r="1" spans="1:5" ht="17.25" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -1608,7 +1687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" thickBot="1">
+    <row r="2" spans="1:5" ht="17.25" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1620,7 +1699,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="27" thickBot="1">
+    <row r="3" spans="1:5" ht="26.25" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1632,7 +1711,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.8" thickBot="1">
+    <row r="4" spans="1:5" ht="27.75" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -1644,7 +1723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="54.6" thickBot="1">
+    <row r="5" spans="1:5" ht="39.75" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
@@ -1656,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.8" thickBot="1">
+    <row r="6" spans="1:5" ht="27.75" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -1668,7 +1747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.8" thickBot="1">
+    <row r="7" spans="1:5" ht="27.75" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1680,7 +1759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.8" thickBot="1">
+    <row r="8" spans="1:5" ht="27.75" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
@@ -1692,7 +1771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="40.200000000000003" thickBot="1">
+    <row r="9" spans="1:5" ht="26.25" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1704,7 +1783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" thickBot="1">
+    <row r="10" spans="1:5" ht="40.5" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
@@ -1715,10 +1794,10 @@
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="31.8" thickBot="1">
+    <row r="11" spans="1:5" ht="27.75" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
@@ -1730,7 +1809,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.8" thickBot="1">
+    <row r="12" spans="1:5" ht="27.75" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>24</v>
       </c>
@@ -1741,7 +1820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.8" thickBot="1">
+    <row r="13" spans="1:5" ht="27.75" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>25</v>
       </c>

</xml_diff>